<commit_message>
Revised training data analysis
Separated balanced, imbalanced, & inadequate data. Separated binary and multi-class problems.
</commit_message>
<xml_diff>
--- a/literature/Plant Disease Detection.xlsx
+++ b/literature/Plant Disease Detection.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8790"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8790" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
   <si>
     <t>YEAR</t>
   </si>
@@ -199,6 +199,21 @@
 ACO was used for feature extraction.
 CNN was used for classification.</t>
     </r>
+  </si>
+  <si>
+    <t>Inadequate data</t>
+  </si>
+  <si>
+    <t>H/D ratio</t>
+  </si>
+  <si>
+    <t>Balanced (binary class)</t>
+  </si>
+  <si>
+    <t>Imbalanced (multi class)</t>
+  </si>
+  <si>
+    <t>#classes</t>
   </si>
 </sst>
 </file>
@@ -299,7 +314,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,8 +345,74 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -382,11 +463,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -418,11 +512,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -439,17 +528,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -463,7 +541,6 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -476,6 +553,60 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,7 +827,7 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -707,7 +838,7 @@
     <col min="3" max="3" width="59" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -719,13 +850,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="280.5">
-      <c r="A2" s="41">
+      <c r="A2" s="32">
         <v>2023</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="33" t="s">
         <v>49</v>
       </c>
     </row>
@@ -733,7 +864,7 @@
       <c r="A3" s="2">
         <v>2022</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="30" t="s">
         <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -750,10 +881,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -763,1107 +894,1220 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12.75">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="73.5" customHeight="1">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17" t="s">
+    <row r="2" spans="1:15" ht="12.75">
+      <c r="A2" s="54"/>
+      <c r="B2" s="18"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1">
+      <c r="B3" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+    </row>
+    <row r="4" spans="1:15" ht="73.5" customHeight="1">
+      <c r="A4" s="16"/>
+      <c r="B4" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="31" t="s">
+      <c r="K4" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="31" t="s">
+      <c r="M4" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="31" t="s">
+      <c r="N4" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="37" t="s">
         <v>16</v>
-      </c>
-      <c r="O3" s="31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="32">
-        <v>1741</v>
-      </c>
-      <c r="C4" s="18">
-        <v>0</v>
-      </c>
-      <c r="D4" s="36">
-        <v>0</v>
-      </c>
-      <c r="E4" s="18">
-        <v>0</v>
-      </c>
-      <c r="F4" s="18">
-        <v>0</v>
-      </c>
-      <c r="G4" s="18">
-        <v>0</v>
-      </c>
-      <c r="H4" s="18">
-        <v>0</v>
-      </c>
-      <c r="I4" s="18">
-        <v>0</v>
-      </c>
-      <c r="J4" s="19">
-        <v>0</v>
-      </c>
-      <c r="K4" s="22">
-        <v>0</v>
-      </c>
-      <c r="L4" s="19">
-        <v>0</v>
-      </c>
-      <c r="M4" s="22">
-        <v>0</v>
-      </c>
-      <c r="N4" s="22">
-        <v>0</v>
-      </c>
-      <c r="O4" s="22">
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="32">
-        <v>1920</v>
-      </c>
-      <c r="C5" s="18">
-        <v>0</v>
-      </c>
-      <c r="D5" s="36">
-        <v>0</v>
-      </c>
-      <c r="E5" s="18">
-        <v>0</v>
-      </c>
-      <c r="F5" s="18">
-        <v>0</v>
-      </c>
-      <c r="G5" s="19">
-        <v>0</v>
-      </c>
-      <c r="H5" s="32">
-        <v>1939</v>
-      </c>
-      <c r="I5" s="18">
-        <v>0</v>
-      </c>
-      <c r="J5" s="19">
-        <v>0</v>
-      </c>
-      <c r="K5" s="22">
-        <v>0</v>
-      </c>
-      <c r="L5" s="19">
-        <v>0</v>
-      </c>
-      <c r="M5" s="22">
-        <v>0</v>
-      </c>
-      <c r="N5" s="22">
-        <v>0</v>
-      </c>
-      <c r="O5" s="22">
+        <v>18</v>
+      </c>
+      <c r="B5" s="45">
+        <v>0</v>
+      </c>
+      <c r="C5" s="46">
+        <v>0</v>
+      </c>
+      <c r="D5" s="46">
+        <v>0</v>
+      </c>
+      <c r="E5" s="46">
+        <v>0</v>
+      </c>
+      <c r="F5" s="48">
+        <v>0</v>
+      </c>
+      <c r="G5" s="49">
+        <v>0</v>
+      </c>
+      <c r="H5" s="48">
+        <v>0</v>
+      </c>
+      <c r="I5" s="48">
+        <v>0</v>
+      </c>
+      <c r="J5" s="50">
+        <v>1741</v>
+      </c>
+      <c r="K5" s="19">
+        <v>0</v>
+      </c>
+      <c r="L5" s="28">
+        <v>0</v>
+      </c>
+      <c r="M5" s="19">
+        <v>0</v>
+      </c>
+      <c r="N5" s="19">
+        <v>0</v>
+      </c>
+      <c r="O5" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="32">
-        <v>1702</v>
-      </c>
-      <c r="C6" s="18">
-        <v>0</v>
-      </c>
-      <c r="D6" s="36">
-        <v>0</v>
-      </c>
-      <c r="E6" s="19">
-        <v>0</v>
-      </c>
-      <c r="F6" s="32">
-        <v>1838</v>
-      </c>
-      <c r="G6" s="18">
-        <v>0</v>
-      </c>
-      <c r="H6" s="18">
-        <v>0</v>
-      </c>
-      <c r="I6" s="18">
-        <v>0</v>
-      </c>
-      <c r="J6" s="19">
-        <v>0</v>
-      </c>
-      <c r="K6" s="22">
-        <v>0</v>
-      </c>
-      <c r="L6" s="32">
-        <v>1913</v>
-      </c>
-      <c r="M6" s="22">
-        <v>0</v>
-      </c>
-      <c r="N6" s="22">
-        <v>0</v>
-      </c>
-      <c r="O6" s="22">
+        <v>19</v>
+      </c>
+      <c r="B6" s="45">
+        <v>0</v>
+      </c>
+      <c r="C6" s="46">
+        <v>0</v>
+      </c>
+      <c r="D6" s="45">
+        <v>0</v>
+      </c>
+      <c r="E6" s="46">
+        <v>0</v>
+      </c>
+      <c r="F6" s="48">
+        <v>0</v>
+      </c>
+      <c r="G6" s="49">
+        <v>0</v>
+      </c>
+      <c r="H6" s="48">
+        <v>0</v>
+      </c>
+      <c r="I6" s="50">
+        <v>1939</v>
+      </c>
+      <c r="J6" s="50">
+        <v>1920</v>
+      </c>
+      <c r="K6" s="19">
+        <v>0</v>
+      </c>
+      <c r="L6" s="28">
+        <v>0</v>
+      </c>
+      <c r="M6" s="19">
+        <v>0</v>
+      </c>
+      <c r="N6" s="19">
+        <v>0</v>
+      </c>
+      <c r="O6" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="19">
-        <v>0</v>
-      </c>
-      <c r="C7" s="32">
-        <v>1683</v>
-      </c>
-      <c r="D7" s="36">
-        <v>0</v>
-      </c>
-      <c r="E7" s="18">
-        <v>0</v>
-      </c>
-      <c r="F7" s="18">
-        <v>0</v>
-      </c>
-      <c r="G7" s="18">
-        <v>0</v>
-      </c>
-      <c r="H7" s="18">
-        <v>0</v>
-      </c>
-      <c r="I7" s="18">
-        <v>0</v>
-      </c>
-      <c r="J7" s="19">
-        <v>0</v>
-      </c>
-      <c r="K7" s="22">
-        <v>0</v>
-      </c>
-      <c r="L7" s="19">
-        <v>0</v>
-      </c>
-      <c r="M7" s="22">
-        <v>0</v>
-      </c>
-      <c r="N7" s="33">
-        <v>1736</v>
-      </c>
-      <c r="O7" s="22">
+        <v>20</v>
+      </c>
+      <c r="B7" s="47">
+        <v>1913</v>
+      </c>
+      <c r="C7" s="46">
+        <v>0</v>
+      </c>
+      <c r="D7" s="46">
+        <v>0</v>
+      </c>
+      <c r="E7" s="47">
+        <v>1838</v>
+      </c>
+      <c r="F7" s="49">
+        <v>0</v>
+      </c>
+      <c r="G7" s="49">
+        <v>0</v>
+      </c>
+      <c r="H7" s="48">
+        <v>0</v>
+      </c>
+      <c r="I7" s="48">
+        <v>0</v>
+      </c>
+      <c r="J7" s="50">
+        <v>1702</v>
+      </c>
+      <c r="K7" s="19">
+        <v>0</v>
+      </c>
+      <c r="L7" s="28">
+        <v>0</v>
+      </c>
+      <c r="M7" s="19">
+        <v>0</v>
+      </c>
+      <c r="N7" s="19">
+        <v>0</v>
+      </c>
+      <c r="O7" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="18">
-        <v>0</v>
-      </c>
-      <c r="C8" s="18">
-        <v>0</v>
-      </c>
-      <c r="D8" s="22">
-        <v>0</v>
-      </c>
-      <c r="E8" s="32">
-        <v>1987</v>
-      </c>
-      <c r="F8" s="18">
-        <v>0</v>
-      </c>
-      <c r="G8" s="18">
-        <v>0</v>
-      </c>
-      <c r="H8" s="19">
-        <v>0</v>
-      </c>
-      <c r="I8" s="32">
-        <v>1888</v>
-      </c>
-      <c r="J8" s="19">
-        <v>0</v>
-      </c>
-      <c r="K8" s="22">
-        <v>0</v>
-      </c>
-      <c r="L8" s="19">
-        <v>0</v>
-      </c>
-      <c r="M8" s="22">
-        <v>0</v>
-      </c>
-      <c r="N8" s="22">
-        <v>0</v>
-      </c>
-      <c r="O8" s="22">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="B8" s="45">
+        <v>0</v>
+      </c>
+      <c r="C8" s="47">
+        <v>1683</v>
+      </c>
+      <c r="D8" s="46">
+        <v>0</v>
+      </c>
+      <c r="E8" s="46">
+        <v>0</v>
+      </c>
+      <c r="F8" s="48">
+        <v>0</v>
+      </c>
+      <c r="G8" s="49">
+        <v>0</v>
+      </c>
+      <c r="H8" s="48">
+        <v>0</v>
+      </c>
+      <c r="I8" s="48">
+        <v>0</v>
+      </c>
+      <c r="J8" s="49">
+        <v>0</v>
+      </c>
+      <c r="K8" s="19">
+        <v>0</v>
+      </c>
+      <c r="L8" s="28">
+        <v>0</v>
+      </c>
+      <c r="M8" s="19">
+        <v>0</v>
+      </c>
+      <c r="N8" s="19">
+        <v>0</v>
+      </c>
+      <c r="O8" s="25">
+        <v>1736</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="32">
-        <v>1790</v>
-      </c>
-      <c r="C9" s="18">
-        <v>0</v>
-      </c>
-      <c r="D9" s="36">
-        <v>0</v>
-      </c>
-      <c r="E9" s="18">
-        <v>0</v>
-      </c>
-      <c r="F9" s="18">
-        <v>0</v>
-      </c>
-      <c r="G9" s="18">
-        <v>0</v>
-      </c>
-      <c r="H9" s="18">
-        <v>0</v>
-      </c>
-      <c r="I9" s="18">
-        <v>0</v>
-      </c>
-      <c r="J9" s="19">
-        <v>0</v>
-      </c>
-      <c r="K9" s="22">
+        <v>22</v>
+      </c>
+      <c r="B9" s="45">
+        <v>0</v>
+      </c>
+      <c r="C9" s="46">
+        <v>0</v>
+      </c>
+      <c r="D9" s="46">
+        <v>0</v>
+      </c>
+      <c r="E9" s="46">
+        <v>0</v>
+      </c>
+      <c r="F9" s="50">
+        <v>1987</v>
+      </c>
+      <c r="G9" s="49">
+        <v>0</v>
+      </c>
+      <c r="H9" s="50">
+        <v>1888</v>
+      </c>
+      <c r="I9" s="49">
+        <v>0</v>
+      </c>
+      <c r="J9" s="48">
+        <v>0</v>
+      </c>
+      <c r="K9" s="19">
         <v>0</v>
       </c>
       <c r="L9" s="19">
         <v>0</v>
       </c>
-      <c r="M9" s="22">
-        <v>0</v>
-      </c>
-      <c r="N9" s="22">
-        <v>0</v>
-      </c>
-      <c r="O9" s="22">
+      <c r="M9" s="19">
+        <v>0</v>
+      </c>
+      <c r="N9" s="19">
+        <v>0</v>
+      </c>
+      <c r="O9" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="18">
-        <v>0</v>
-      </c>
-      <c r="C10" s="18">
-        <v>0</v>
-      </c>
-      <c r="D10" s="36">
-        <v>0</v>
-      </c>
-      <c r="E10" s="18">
-        <v>0</v>
-      </c>
-      <c r="F10" s="19">
-        <v>0</v>
-      </c>
-      <c r="G10" s="32">
-        <v>1774</v>
-      </c>
-      <c r="H10" s="18">
-        <v>0</v>
-      </c>
-      <c r="I10" s="18">
-        <v>0</v>
-      </c>
-      <c r="J10" s="19">
-        <v>0</v>
-      </c>
-      <c r="K10" s="22">
-        <v>0</v>
-      </c>
-      <c r="L10" s="19">
-        <v>0</v>
-      </c>
-      <c r="M10" s="22">
-        <v>0</v>
-      </c>
-      <c r="N10" s="22">
-        <v>0</v>
-      </c>
-      <c r="O10" s="22">
+        <v>23</v>
+      </c>
+      <c r="B10" s="45">
+        <v>0</v>
+      </c>
+      <c r="C10" s="46">
+        <v>0</v>
+      </c>
+      <c r="D10" s="46">
+        <v>0</v>
+      </c>
+      <c r="E10" s="46">
+        <v>0</v>
+      </c>
+      <c r="F10" s="48">
+        <v>0</v>
+      </c>
+      <c r="G10" s="49">
+        <v>0</v>
+      </c>
+      <c r="H10" s="48">
+        <v>0</v>
+      </c>
+      <c r="I10" s="48">
+        <v>0</v>
+      </c>
+      <c r="J10" s="50">
+        <v>1790</v>
+      </c>
+      <c r="K10" s="19">
+        <v>0</v>
+      </c>
+      <c r="L10" s="28">
+        <v>0</v>
+      </c>
+      <c r="M10" s="19">
+        <v>0</v>
+      </c>
+      <c r="N10" s="19">
+        <v>0</v>
+      </c>
+      <c r="O10" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="18">
-        <v>0</v>
-      </c>
-      <c r="C11" s="18">
-        <v>0</v>
-      </c>
-      <c r="D11" s="22">
-        <v>0</v>
-      </c>
-      <c r="E11" s="32">
-        <v>2016</v>
-      </c>
-      <c r="F11" s="18">
-        <v>0</v>
-      </c>
-      <c r="G11" s="18">
-        <v>0</v>
-      </c>
-      <c r="H11" s="18">
-        <v>0</v>
-      </c>
-      <c r="I11" s="18">
-        <v>0</v>
-      </c>
-      <c r="J11" s="19">
-        <v>0</v>
-      </c>
-      <c r="K11" s="22">
-        <v>0</v>
-      </c>
-      <c r="L11" s="19">
-        <v>0</v>
-      </c>
-      <c r="M11" s="22">
-        <v>0</v>
-      </c>
-      <c r="N11" s="22">
-        <v>0</v>
-      </c>
-      <c r="O11" s="22">
+        <v>24</v>
+      </c>
+      <c r="B11" s="45">
+        <v>0</v>
+      </c>
+      <c r="C11" s="46">
+        <v>0</v>
+      </c>
+      <c r="D11" s="47">
+        <v>1774</v>
+      </c>
+      <c r="E11" s="45">
+        <v>0</v>
+      </c>
+      <c r="F11" s="48">
+        <v>0</v>
+      </c>
+      <c r="G11" s="49">
+        <v>0</v>
+      </c>
+      <c r="H11" s="48">
+        <v>0</v>
+      </c>
+      <c r="I11" s="48">
+        <v>0</v>
+      </c>
+      <c r="J11" s="48">
+        <v>0</v>
+      </c>
+      <c r="K11" s="19">
+        <v>0</v>
+      </c>
+      <c r="L11" s="28">
+        <v>0</v>
+      </c>
+      <c r="M11" s="19">
+        <v>0</v>
+      </c>
+      <c r="N11" s="19">
+        <v>0</v>
+      </c>
+      <c r="O11" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="18">
-        <v>0</v>
-      </c>
-      <c r="C12" s="18">
-        <v>0</v>
-      </c>
-      <c r="D12" s="36">
-        <v>0</v>
-      </c>
-      <c r="E12" s="18">
-        <v>0</v>
-      </c>
-      <c r="F12" s="18">
-        <v>0</v>
-      </c>
-      <c r="G12" s="18">
-        <v>0</v>
-      </c>
-      <c r="H12" s="19">
-        <v>0</v>
-      </c>
-      <c r="I12" s="32">
-        <v>1722</v>
-      </c>
-      <c r="J12" s="19">
-        <v>0</v>
-      </c>
-      <c r="K12" s="22">
+        <v>25</v>
+      </c>
+      <c r="B12" s="45">
+        <v>0</v>
+      </c>
+      <c r="C12" s="46">
+        <v>0</v>
+      </c>
+      <c r="D12" s="46">
+        <v>0</v>
+      </c>
+      <c r="E12" s="46">
+        <v>0</v>
+      </c>
+      <c r="F12" s="50">
+        <v>2016</v>
+      </c>
+      <c r="G12" s="49">
+        <v>0</v>
+      </c>
+      <c r="H12" s="48">
+        <v>0</v>
+      </c>
+      <c r="I12" s="48">
+        <v>0</v>
+      </c>
+      <c r="J12" s="48">
+        <v>0</v>
+      </c>
+      <c r="K12" s="19">
         <v>0</v>
       </c>
       <c r="L12" s="19">
         <v>0</v>
       </c>
-      <c r="M12" s="22">
-        <v>0</v>
-      </c>
-      <c r="N12" s="22">
-        <v>0</v>
-      </c>
-      <c r="O12" s="22">
+      <c r="M12" s="19">
+        <v>0</v>
+      </c>
+      <c r="N12" s="19">
+        <v>0</v>
+      </c>
+      <c r="O12" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="18">
-        <v>0</v>
-      </c>
-      <c r="C13" s="18">
-        <v>0</v>
-      </c>
-      <c r="D13" s="36">
-        <v>0</v>
-      </c>
-      <c r="E13" s="18">
-        <v>0</v>
-      </c>
-      <c r="F13" s="18">
-        <v>0</v>
-      </c>
-      <c r="G13" s="18">
-        <v>0</v>
-      </c>
-      <c r="H13" s="18">
-        <v>0</v>
-      </c>
-      <c r="I13" s="19">
-        <v>0</v>
-      </c>
-      <c r="J13" s="32">
-        <v>1907</v>
-      </c>
-      <c r="K13" s="22">
-        <v>0</v>
-      </c>
-      <c r="L13" s="19">
-        <v>0</v>
-      </c>
-      <c r="M13" s="22">
-        <v>0</v>
-      </c>
-      <c r="N13" s="22">
-        <v>0</v>
-      </c>
-      <c r="O13" s="22">
+        <v>26</v>
+      </c>
+      <c r="B13" s="45">
+        <v>0</v>
+      </c>
+      <c r="C13" s="46">
+        <v>0</v>
+      </c>
+      <c r="D13" s="46">
+        <v>0</v>
+      </c>
+      <c r="E13" s="46">
+        <v>0</v>
+      </c>
+      <c r="F13" s="48">
+        <v>0</v>
+      </c>
+      <c r="G13" s="49">
+        <v>0</v>
+      </c>
+      <c r="H13" s="50">
+        <v>1722</v>
+      </c>
+      <c r="I13" s="49">
+        <v>0</v>
+      </c>
+      <c r="J13" s="48">
+        <v>0</v>
+      </c>
+      <c r="K13" s="19">
+        <v>0</v>
+      </c>
+      <c r="L13" s="28">
+        <v>0</v>
+      </c>
+      <c r="M13" s="19">
+        <v>0</v>
+      </c>
+      <c r="N13" s="19">
+        <v>0</v>
+      </c>
+      <c r="O13" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="32">
-        <v>1827</v>
-      </c>
-      <c r="C14" s="18">
-        <v>0</v>
-      </c>
-      <c r="D14" s="36">
-        <v>0</v>
-      </c>
-      <c r="E14" s="18">
-        <v>0</v>
-      </c>
-      <c r="F14" s="18">
-        <v>0</v>
-      </c>
-      <c r="G14" s="18">
-        <v>0</v>
-      </c>
-      <c r="H14" s="18">
-        <v>0</v>
-      </c>
-      <c r="I14" s="18">
-        <v>0</v>
-      </c>
-      <c r="J14" s="19">
-        <v>0</v>
-      </c>
-      <c r="K14" s="22">
-        <v>0</v>
-      </c>
-      <c r="L14" s="19">
-        <v>0</v>
-      </c>
-      <c r="M14" s="22">
-        <v>0</v>
-      </c>
-      <c r="N14" s="22">
-        <v>0</v>
-      </c>
-      <c r="O14" s="22">
+        <v>27</v>
+      </c>
+      <c r="B14" s="45">
+        <v>0</v>
+      </c>
+      <c r="C14" s="46">
+        <v>0</v>
+      </c>
+      <c r="D14" s="46">
+        <v>0</v>
+      </c>
+      <c r="E14" s="46">
+        <v>0</v>
+      </c>
+      <c r="F14" s="48">
+        <v>0</v>
+      </c>
+      <c r="G14" s="50">
+        <v>1907</v>
+      </c>
+      <c r="H14" s="49">
+        <v>0</v>
+      </c>
+      <c r="I14" s="48">
+        <v>0</v>
+      </c>
+      <c r="J14" s="48">
+        <v>0</v>
+      </c>
+      <c r="K14" s="19">
+        <v>0</v>
+      </c>
+      <c r="L14" s="28">
+        <v>0</v>
+      </c>
+      <c r="M14" s="19">
+        <v>0</v>
+      </c>
+      <c r="N14" s="19">
+        <v>0</v>
+      </c>
+      <c r="O14" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="18">
-        <v>0</v>
-      </c>
-      <c r="C15" s="18">
-        <v>0</v>
-      </c>
-      <c r="D15" s="36">
-        <v>0</v>
-      </c>
-      <c r="E15" s="18">
-        <v>0</v>
-      </c>
-      <c r="F15" s="18">
-        <v>0</v>
-      </c>
-      <c r="G15" s="18">
-        <v>0</v>
-      </c>
-      <c r="H15" s="18">
-        <v>0</v>
-      </c>
-      <c r="I15" s="19">
-        <v>0</v>
-      </c>
-      <c r="J15" s="32">
-        <v>1908</v>
-      </c>
-      <c r="K15" s="22">
-        <v>0</v>
-      </c>
-      <c r="L15" s="19">
-        <v>0</v>
-      </c>
-      <c r="M15" s="22">
-        <v>0</v>
-      </c>
-      <c r="N15" s="22">
-        <v>0</v>
-      </c>
-      <c r="O15" s="22">
+        <v>28</v>
+      </c>
+      <c r="B15" s="45">
+        <v>0</v>
+      </c>
+      <c r="C15" s="46">
+        <v>0</v>
+      </c>
+      <c r="D15" s="46">
+        <v>0</v>
+      </c>
+      <c r="E15" s="46">
+        <v>0</v>
+      </c>
+      <c r="F15" s="48">
+        <v>0</v>
+      </c>
+      <c r="G15" s="49">
+        <v>0</v>
+      </c>
+      <c r="H15" s="48">
+        <v>0</v>
+      </c>
+      <c r="I15" s="48">
+        <v>0</v>
+      </c>
+      <c r="J15" s="50">
+        <v>1827</v>
+      </c>
+      <c r="K15" s="19">
+        <v>0</v>
+      </c>
+      <c r="L15" s="28">
+        <v>0</v>
+      </c>
+      <c r="M15" s="19">
+        <v>0</v>
+      </c>
+      <c r="N15" s="19">
+        <v>0</v>
+      </c>
+      <c r="O15" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="18">
-        <v>0</v>
-      </c>
-      <c r="C16" s="18">
-        <v>0</v>
-      </c>
-      <c r="D16" s="36">
-        <v>0</v>
-      </c>
-      <c r="E16" s="18">
-        <v>0</v>
-      </c>
-      <c r="F16" s="18">
-        <v>0</v>
-      </c>
-      <c r="G16" s="18">
-        <v>0</v>
-      </c>
-      <c r="H16" s="18">
-        <v>0</v>
-      </c>
-      <c r="I16" s="19">
-        <v>0</v>
-      </c>
-      <c r="J16" s="32">
-        <v>1642</v>
-      </c>
-      <c r="K16" s="22">
-        <v>0</v>
-      </c>
-      <c r="L16" s="19">
-        <v>0</v>
-      </c>
-      <c r="M16" s="22">
-        <v>0</v>
-      </c>
-      <c r="N16" s="22">
-        <v>0</v>
-      </c>
-      <c r="O16" s="22">
+        <v>29</v>
+      </c>
+      <c r="B16" s="45">
+        <v>0</v>
+      </c>
+      <c r="C16" s="46">
+        <v>0</v>
+      </c>
+      <c r="D16" s="46">
+        <v>0</v>
+      </c>
+      <c r="E16" s="46">
+        <v>0</v>
+      </c>
+      <c r="F16" s="48">
+        <v>0</v>
+      </c>
+      <c r="G16" s="50">
+        <v>1908</v>
+      </c>
+      <c r="H16" s="49">
+        <v>0</v>
+      </c>
+      <c r="I16" s="48">
+        <v>0</v>
+      </c>
+      <c r="J16" s="48">
+        <v>0</v>
+      </c>
+      <c r="K16" s="19">
+        <v>0</v>
+      </c>
+      <c r="L16" s="28">
+        <v>0</v>
+      </c>
+      <c r="M16" s="19">
+        <v>0</v>
+      </c>
+      <c r="N16" s="19">
+        <v>0</v>
+      </c>
+      <c r="O16" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="32">
-        <v>1882</v>
-      </c>
-      <c r="C17" s="32">
-        <v>0</v>
-      </c>
-      <c r="D17" s="33">
-        <v>0</v>
-      </c>
-      <c r="E17" s="32">
-        <v>0</v>
-      </c>
-      <c r="F17" s="32">
-        <v>0</v>
-      </c>
-      <c r="G17" s="19">
-        <v>0</v>
-      </c>
-      <c r="H17" s="32">
-        <v>0</v>
-      </c>
-      <c r="I17" s="19">
-        <v>0</v>
-      </c>
-      <c r="J17" s="32">
-        <v>0</v>
-      </c>
-      <c r="K17" s="33">
-        <v>0</v>
-      </c>
-      <c r="L17" s="19">
-        <v>0</v>
-      </c>
-      <c r="M17" s="33">
-        <v>0</v>
-      </c>
-      <c r="N17" s="22">
-        <v>0</v>
-      </c>
-      <c r="O17" s="22">
+        <v>30</v>
+      </c>
+      <c r="B17" s="45">
+        <v>0</v>
+      </c>
+      <c r="C17" s="46">
+        <v>0</v>
+      </c>
+      <c r="D17" s="46">
+        <v>0</v>
+      </c>
+      <c r="E17" s="46">
+        <v>0</v>
+      </c>
+      <c r="F17" s="48">
+        <v>0</v>
+      </c>
+      <c r="G17" s="50">
+        <v>1642</v>
+      </c>
+      <c r="H17" s="49">
+        <v>0</v>
+      </c>
+      <c r="I17" s="48">
+        <v>0</v>
+      </c>
+      <c r="J17" s="48">
+        <v>0</v>
+      </c>
+      <c r="K17" s="19">
+        <v>0</v>
+      </c>
+      <c r="L17" s="28">
+        <v>0</v>
+      </c>
+      <c r="M17" s="19">
+        <v>0</v>
+      </c>
+      <c r="N17" s="19">
+        <v>0</v>
+      </c>
+      <c r="O17" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1">
       <c r="A18" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="32">
-        <v>1745</v>
-      </c>
-      <c r="C18" s="32">
-        <v>0</v>
-      </c>
-      <c r="D18" s="33">
-        <v>0</v>
-      </c>
-      <c r="E18" s="32">
-        <v>0</v>
-      </c>
-      <c r="F18" s="32">
-        <v>0</v>
-      </c>
-      <c r="G18" s="19">
-        <v>0</v>
-      </c>
-      <c r="H18" s="32">
-        <v>0</v>
-      </c>
-      <c r="I18" s="19">
-        <v>0</v>
-      </c>
-      <c r="J18" s="32">
-        <v>0</v>
-      </c>
-      <c r="K18" s="33">
-        <v>0</v>
-      </c>
-      <c r="L18" s="19">
-        <v>0</v>
-      </c>
-      <c r="M18" s="33">
-        <v>0</v>
-      </c>
-      <c r="N18" s="22">
-        <v>0</v>
-      </c>
-      <c r="O18" s="22">
+        <v>31</v>
+      </c>
+      <c r="B18" s="45">
+        <v>0</v>
+      </c>
+      <c r="C18" s="47">
+        <v>0</v>
+      </c>
+      <c r="D18" s="45">
+        <v>0</v>
+      </c>
+      <c r="E18" s="47">
+        <v>0</v>
+      </c>
+      <c r="F18" s="50">
+        <v>0</v>
+      </c>
+      <c r="G18" s="50">
+        <v>0</v>
+      </c>
+      <c r="H18" s="49">
+        <v>0</v>
+      </c>
+      <c r="I18" s="50">
+        <v>0</v>
+      </c>
+      <c r="J18" s="50">
+        <v>1882</v>
+      </c>
+      <c r="K18" s="25">
+        <v>0</v>
+      </c>
+      <c r="L18" s="25">
+        <v>0</v>
+      </c>
+      <c r="M18" s="25">
+        <v>0</v>
+      </c>
+      <c r="N18" s="19">
+        <v>0</v>
+      </c>
+      <c r="O18" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1">
       <c r="A19" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="19">
-        <v>0</v>
-      </c>
-      <c r="C19" s="32">
-        <v>0</v>
-      </c>
-      <c r="D19" s="33">
-        <v>0</v>
-      </c>
-      <c r="E19" s="32">
-        <v>1760</v>
-      </c>
-      <c r="F19" s="32">
-        <v>0</v>
-      </c>
-      <c r="G19" s="19">
-        <v>0</v>
-      </c>
-      <c r="H19" s="32">
-        <v>0</v>
-      </c>
-      <c r="I19" s="19">
-        <v>0</v>
-      </c>
-      <c r="J19" s="32">
-        <v>0</v>
-      </c>
-      <c r="K19" s="33">
-        <v>0</v>
-      </c>
-      <c r="L19" s="19">
-        <v>0</v>
-      </c>
-      <c r="M19" s="33">
-        <v>0</v>
-      </c>
-      <c r="N19" s="22">
-        <v>0</v>
-      </c>
-      <c r="O19" s="22">
+        <v>32</v>
+      </c>
+      <c r="B19" s="45">
+        <v>0</v>
+      </c>
+      <c r="C19" s="47">
+        <v>0</v>
+      </c>
+      <c r="D19" s="45">
+        <v>0</v>
+      </c>
+      <c r="E19" s="47">
+        <v>0</v>
+      </c>
+      <c r="F19" s="50">
+        <v>0</v>
+      </c>
+      <c r="G19" s="50">
+        <v>0</v>
+      </c>
+      <c r="H19" s="49">
+        <v>0</v>
+      </c>
+      <c r="I19" s="50">
+        <v>0</v>
+      </c>
+      <c r="J19" s="50">
+        <v>1745</v>
+      </c>
+      <c r="K19" s="25">
+        <v>0</v>
+      </c>
+      <c r="L19" s="25">
+        <v>0</v>
+      </c>
+      <c r="M19" s="25">
+        <v>0</v>
+      </c>
+      <c r="N19" s="19">
+        <v>0</v>
+      </c>
+      <c r="O19" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1">
       <c r="A20" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="32">
-        <v>1961</v>
-      </c>
-      <c r="C20" s="32">
-        <v>0</v>
-      </c>
-      <c r="D20" s="33">
-        <v>0</v>
-      </c>
-      <c r="E20" s="32">
-        <v>0</v>
-      </c>
-      <c r="F20" s="32">
-        <v>0</v>
-      </c>
-      <c r="G20" s="19">
-        <v>0</v>
-      </c>
-      <c r="H20" s="32">
-        <v>0</v>
-      </c>
-      <c r="I20" s="19">
-        <v>0</v>
-      </c>
-      <c r="J20" s="32">
-        <v>0</v>
-      </c>
-      <c r="K20" s="33">
-        <v>0</v>
-      </c>
-      <c r="L20" s="19">
-        <v>0</v>
-      </c>
-      <c r="M20" s="33">
-        <v>0</v>
-      </c>
-      <c r="N20" s="22">
-        <v>0</v>
-      </c>
-      <c r="O20" s="22">
+        <v>33</v>
+      </c>
+      <c r="B20" s="45">
+        <v>0</v>
+      </c>
+      <c r="C20" s="47">
+        <v>0</v>
+      </c>
+      <c r="D20" s="45">
+        <v>0</v>
+      </c>
+      <c r="E20" s="47">
+        <v>0</v>
+      </c>
+      <c r="F20" s="50">
+        <v>1760</v>
+      </c>
+      <c r="G20" s="50">
+        <v>0</v>
+      </c>
+      <c r="H20" s="49">
+        <v>0</v>
+      </c>
+      <c r="I20" s="50">
+        <v>0</v>
+      </c>
+      <c r="J20" s="49">
+        <v>0</v>
+      </c>
+      <c r="K20" s="25">
+        <v>0</v>
+      </c>
+      <c r="L20" s="25">
+        <v>0</v>
+      </c>
+      <c r="M20" s="25">
+        <v>0</v>
+      </c>
+      <c r="N20" s="19">
+        <v>0</v>
+      </c>
+      <c r="O20" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1">
       <c r="A21" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="19">
-        <v>0</v>
-      </c>
-      <c r="C21" s="32">
-        <v>0</v>
-      </c>
-      <c r="D21" s="33">
-        <v>0</v>
-      </c>
-      <c r="E21" s="32">
-        <v>0</v>
-      </c>
-      <c r="F21" s="32">
-        <v>0</v>
-      </c>
-      <c r="G21" s="19">
-        <v>0</v>
-      </c>
-      <c r="H21" s="32">
-        <v>0</v>
-      </c>
-      <c r="I21" s="32">
-        <v>1920</v>
-      </c>
-      <c r="J21" s="32">
-        <v>0</v>
-      </c>
-      <c r="K21" s="33">
-        <v>0</v>
-      </c>
-      <c r="L21" s="19">
-        <v>0</v>
-      </c>
-      <c r="M21" s="33">
-        <v>0</v>
-      </c>
-      <c r="N21" s="22">
-        <v>0</v>
-      </c>
-      <c r="O21" s="22">
+        <v>34</v>
+      </c>
+      <c r="B21" s="45">
+        <v>0</v>
+      </c>
+      <c r="C21" s="47">
+        <v>0</v>
+      </c>
+      <c r="D21" s="45">
+        <v>0</v>
+      </c>
+      <c r="E21" s="47">
+        <v>0</v>
+      </c>
+      <c r="F21" s="50">
+        <v>0</v>
+      </c>
+      <c r="G21" s="50">
+        <v>0</v>
+      </c>
+      <c r="H21" s="49">
+        <v>0</v>
+      </c>
+      <c r="I21" s="50">
+        <v>0</v>
+      </c>
+      <c r="J21" s="50">
+        <v>1961</v>
+      </c>
+      <c r="K21" s="25">
+        <v>0</v>
+      </c>
+      <c r="L21" s="25">
+        <v>0</v>
+      </c>
+      <c r="M21" s="25">
+        <v>0</v>
+      </c>
+      <c r="N21" s="19">
+        <v>0</v>
+      </c>
+      <c r="O21" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1">
       <c r="A22" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="45">
+        <v>0</v>
+      </c>
+      <c r="C22" s="47">
+        <v>0</v>
+      </c>
+      <c r="D22" s="45">
+        <v>0</v>
+      </c>
+      <c r="E22" s="47">
+        <v>0</v>
+      </c>
+      <c r="F22" s="50">
+        <v>0</v>
+      </c>
+      <c r="G22" s="50">
+        <v>0</v>
+      </c>
+      <c r="H22" s="50">
+        <v>1920</v>
+      </c>
+      <c r="I22" s="50">
+        <v>0</v>
+      </c>
+      <c r="J22" s="49">
+        <v>0</v>
+      </c>
+      <c r="K22" s="25">
+        <v>0</v>
+      </c>
+      <c r="L22" s="25">
+        <v>0</v>
+      </c>
+      <c r="M22" s="25">
+        <v>0</v>
+      </c>
+      <c r="N22" s="19">
+        <v>0</v>
+      </c>
+      <c r="O22" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A23" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="19">
-        <v>0</v>
-      </c>
-      <c r="C22" s="32">
-        <v>0</v>
-      </c>
-      <c r="D22" s="33">
-        <v>0</v>
-      </c>
-      <c r="E22" s="32">
-        <v>0</v>
-      </c>
-      <c r="F22" s="32">
-        <v>0</v>
-      </c>
-      <c r="G22" s="32">
-        <v>0</v>
-      </c>
-      <c r="H22" s="32">
-        <v>0</v>
-      </c>
-      <c r="I22" s="19">
-        <v>0</v>
-      </c>
-      <c r="J22" s="32">
-        <v>0</v>
-      </c>
-      <c r="K22" s="33">
-        <v>0</v>
-      </c>
-      <c r="L22" s="19">
-        <v>0</v>
-      </c>
-      <c r="M22" s="33">
-        <v>0</v>
-      </c>
-      <c r="N22" s="22">
-        <v>0</v>
-      </c>
-      <c r="O22" s="33">
+      <c r="B23" s="56">
+        <v>0</v>
+      </c>
+      <c r="C23" s="57">
+        <v>0</v>
+      </c>
+      <c r="D23" s="57">
+        <v>0</v>
+      </c>
+      <c r="E23" s="57">
+        <v>0</v>
+      </c>
+      <c r="F23" s="58">
+        <v>0</v>
+      </c>
+      <c r="G23" s="58">
+        <v>0</v>
+      </c>
+      <c r="H23" s="59">
+        <v>0</v>
+      </c>
+      <c r="I23" s="58">
+        <v>0</v>
+      </c>
+      <c r="J23" s="59">
+        <v>0</v>
+      </c>
+      <c r="K23" s="25">
+        <v>0</v>
+      </c>
+      <c r="L23" s="25">
+        <v>0</v>
+      </c>
+      <c r="M23" s="25">
+        <v>0</v>
+      </c>
+      <c r="N23" s="25">
         <v>2010</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A23" s="15" t="s">
+      <c r="O23" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A24" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="32">
+      <c r="B24" s="47">
+        <v>0</v>
+      </c>
+      <c r="C24" s="47">
+        <v>0</v>
+      </c>
+      <c r="D24" s="47">
+        <v>0</v>
+      </c>
+      <c r="E24" s="47">
+        <v>0</v>
+      </c>
+      <c r="F24" s="50">
+        <v>0</v>
+      </c>
+      <c r="G24" s="50">
+        <v>0</v>
+      </c>
+      <c r="H24" s="50">
+        <v>0</v>
+      </c>
+      <c r="I24" s="50">
+        <v>1939</v>
+      </c>
+      <c r="J24" s="50">
         <v>1851</v>
       </c>
-      <c r="C23" s="32">
-        <v>0</v>
-      </c>
-      <c r="D23" s="33">
-        <v>0</v>
-      </c>
-      <c r="E23" s="32">
-        <v>0</v>
-      </c>
-      <c r="F23" s="32">
-        <v>0</v>
-      </c>
-      <c r="G23" s="32">
-        <v>0</v>
-      </c>
-      <c r="H23" s="32">
-        <v>1939</v>
-      </c>
-      <c r="I23" s="32">
-        <v>0</v>
-      </c>
-      <c r="J23" s="32">
-        <v>0</v>
-      </c>
-      <c r="K23" s="33">
-        <v>0</v>
-      </c>
-      <c r="L23" s="32">
-        <v>0</v>
-      </c>
-      <c r="M23" s="33">
-        <v>0</v>
-      </c>
-      <c r="N23" s="22">
-        <v>0</v>
-      </c>
-      <c r="O23" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="12.75">
-      <c r="A24" s="27" t="s">
+      <c r="K24" s="25">
+        <v>0</v>
+      </c>
+      <c r="L24" s="25">
+        <v>0</v>
+      </c>
+      <c r="M24" s="25">
+        <v>0</v>
+      </c>
+      <c r="N24" s="19">
+        <v>0</v>
+      </c>
+      <c r="O24" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="12.75">
+      <c r="A25" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="34">
+      <c r="B25" s="26">
+        <v>1988</v>
+      </c>
+      <c r="C25" s="26">
+        <v>1826</v>
+      </c>
+      <c r="D25" s="26">
+        <v>1824</v>
+      </c>
+      <c r="E25" s="26">
+        <v>1728</v>
+      </c>
+      <c r="F25" s="26">
+        <v>2008</v>
+      </c>
+      <c r="G25" s="26">
+        <v>1859</v>
+      </c>
+      <c r="H25" s="26">
+        <v>1692</v>
+      </c>
+      <c r="I25" s="26">
+        <v>1824</v>
+      </c>
+      <c r="J25" s="26">
         <v>1926</v>
       </c>
-      <c r="C24" s="34">
-        <v>1826</v>
-      </c>
-      <c r="D24" s="37">
+      <c r="K25" s="29">
+        <v>1816</v>
+      </c>
+      <c r="L25" s="29">
         <v>1781</v>
       </c>
-      <c r="E24" s="34">
-        <v>2008</v>
-      </c>
-      <c r="F24" s="34">
-        <v>1728</v>
-      </c>
-      <c r="G24" s="34">
-        <v>1824</v>
-      </c>
-      <c r="H24" s="34">
-        <v>1824</v>
-      </c>
-      <c r="I24" s="34">
-        <v>1692</v>
-      </c>
-      <c r="J24" s="34">
-        <v>1859</v>
-      </c>
-      <c r="K24" s="37">
-        <v>1816</v>
-      </c>
-      <c r="L24" s="34">
-        <v>1988</v>
-      </c>
-      <c r="M24" s="37">
+      <c r="M25" s="29">
         <v>2022</v>
       </c>
-      <c r="N24" s="28">
-        <v>0</v>
-      </c>
-      <c r="O24" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A25" s="35" t="s">
+      <c r="N25" s="34">
+        <v>0</v>
+      </c>
+      <c r="O25" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A26" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="29">
-        <f>SUM(B4:B23)</f>
+      <c r="B26" s="42">
+        <f>SUM(B5:B24)</f>
+        <v>1913</v>
+      </c>
+      <c r="C26" s="42">
+        <f t="shared" ref="C26:O26" si="0">SUM(C5:C24)</f>
+        <v>1683</v>
+      </c>
+      <c r="D26" s="42">
+        <f>SUM(D5:D24)</f>
+        <v>1774</v>
+      </c>
+      <c r="E26" s="42">
+        <f>SUM(E5:E24)</f>
+        <v>1838</v>
+      </c>
+      <c r="F26" s="42">
+        <f>SUM(F5:F24)</f>
+        <v>5763</v>
+      </c>
+      <c r="G26" s="42">
+        <f>SUM(G5:G24)</f>
+        <v>5457</v>
+      </c>
+      <c r="H26" s="42">
+        <f>SUM(H5:H24)</f>
+        <v>5530</v>
+      </c>
+      <c r="I26" s="42">
+        <f>SUM(I5:I24)</f>
+        <v>3878</v>
+      </c>
+      <c r="J26" s="42">
+        <f>SUM(J5:J24)</f>
         <v>16419</v>
       </c>
-      <c r="C25" s="29">
-        <f t="shared" ref="C25:O25" si="0">SUM(C4:C23)</f>
-        <v>1683</v>
-      </c>
-      <c r="D25" s="38">
+      <c r="K26" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="29">
+      <c r="L26" s="43">
+        <f>SUM(L5:L24)</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="43">
         <f t="shared" si="0"/>
-        <v>5763</v>
-      </c>
-      <c r="F25" s="29">
-        <f t="shared" si="0"/>
-        <v>1838</v>
-      </c>
-      <c r="G25" s="29">
-        <f t="shared" si="0"/>
-        <v>1774</v>
-      </c>
-      <c r="H25" s="29">
-        <f t="shared" si="0"/>
-        <v>3878</v>
-      </c>
-      <c r="I25" s="29">
-        <f t="shared" si="0"/>
-        <v>5530</v>
-      </c>
-      <c r="J25" s="29">
-        <f t="shared" si="0"/>
-        <v>5457</v>
-      </c>
-      <c r="K25" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="29">
-        <f t="shared" si="0"/>
-        <v>1913</v>
-      </c>
-      <c r="M25" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N25" s="29">
+        <v>0</v>
+      </c>
+      <c r="N26" s="43">
+        <f>SUM(N5:N24)</f>
+        <v>2010</v>
+      </c>
+      <c r="O26" s="43">
         <f t="shared" si="0"/>
         <v>1736</v>
       </c>
-      <c r="O25" s="29">
-        <f t="shared" si="0"/>
-        <v>2010</v>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A27" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="51">
+        <f>ROUND(B25/B26,2)</f>
+        <v>1.04</v>
+      </c>
+      <c r="C27" s="51">
+        <f t="shared" ref="C27:J27" si="1">ROUND(C25/C26,2)</f>
+        <v>1.08</v>
+      </c>
+      <c r="D27" s="51">
+        <f t="shared" si="1"/>
+        <v>1.03</v>
+      </c>
+      <c r="E27" s="51">
+        <f t="shared" si="1"/>
+        <v>0.94</v>
+      </c>
+      <c r="F27" s="52">
+        <f t="shared" si="1"/>
+        <v>0.35</v>
+      </c>
+      <c r="G27" s="52">
+        <f t="shared" si="1"/>
+        <v>0.34</v>
+      </c>
+      <c r="H27" s="52">
+        <f t="shared" si="1"/>
+        <v>0.31</v>
+      </c>
+      <c r="I27" s="52">
+        <f t="shared" si="1"/>
+        <v>0.47</v>
+      </c>
+      <c r="J27" s="52">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A28" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="53">
+        <f>21-COUNTIF(B5:B25,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C28" s="53">
+        <f t="shared" ref="C28:J28" si="2">21-COUNTIF(C5:C25,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D28" s="53">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E28" s="53">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F28" s="53">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G28" s="53">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="H28" s="53">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="I28" s="53">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J28" s="53">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="K3:O3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -1876,7 +2120,7 @@
   </sheetPr>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -2949,132 +3193,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="25"/>
-    </row>
-    <row r="3" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A3" s="24" t="s">
+      <c r="B2" s="22"/>
+    </row>
+    <row r="3" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="25"/>
-    </row>
-    <row r="4" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A4" s="24" t="s">
+      <c r="B3" s="22"/>
+    </row>
+    <row r="4" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="25"/>
-    </row>
-    <row r="5" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A5" s="24" t="s">
+      <c r="B4" s="22"/>
+    </row>
+    <row r="5" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A5" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="25"/>
-    </row>
-    <row r="6" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A6" s="24" t="s">
+      <c r="B5" s="22"/>
+    </row>
+    <row r="6" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A6" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="25"/>
-    </row>
-    <row r="7" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A7" s="24" t="s">
+      <c r="B6" s="22"/>
+    </row>
+    <row r="7" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="25"/>
-    </row>
-    <row r="8" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A8" s="24" t="s">
+      <c r="B7" s="22"/>
+    </row>
+    <row r="8" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="25"/>
-    </row>
-    <row r="9" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A9" s="24" t="s">
+      <c r="B8" s="22"/>
+    </row>
+    <row r="9" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A9" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="25"/>
-    </row>
-    <row r="10" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A10" s="24" t="s">
+      <c r="B9" s="22"/>
+    </row>
+    <row r="10" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="25"/>
-    </row>
-    <row r="11" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A11" s="24" t="s">
+      <c r="B10" s="22"/>
+    </row>
+    <row r="11" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A11" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="25"/>
-    </row>
-    <row r="12" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A12" s="24" t="s">
+      <c r="B11" s="22"/>
+    </row>
+    <row r="12" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A12" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="25"/>
-    </row>
-    <row r="13" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A13" s="24" t="s">
+      <c r="B12" s="22"/>
+    </row>
+    <row r="13" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A13" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="25"/>
-    </row>
-    <row r="14" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A14" s="24" t="s">
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A14" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="25"/>
-    </row>
-    <row r="15" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A15" s="24" t="s">
+      <c r="B14" s="22"/>
+    </row>
+    <row r="15" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A15" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="25"/>
-    </row>
-    <row r="16" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A16" s="24" t="s">
+      <c r="B15" s="22"/>
+    </row>
+    <row r="16" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A16" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="25"/>
-    </row>
-    <row r="17" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A17" s="24" t="s">
+      <c r="B16" s="22"/>
+    </row>
+    <row r="17" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A17" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="25"/>
-    </row>
-    <row r="18" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A18" s="24" t="s">
+      <c r="B17" s="22"/>
+    </row>
+    <row r="18" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A18" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="25"/>
-    </row>
-    <row r="19" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A19" s="24" t="s">
+      <c r="B18" s="22"/>
+    </row>
+    <row r="19" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A19" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="25"/>
-    </row>
-    <row r="20" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A20" s="24" t="s">
+      <c r="B19" s="22"/>
+    </row>
+    <row r="20" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A20" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="25"/>
-    </row>
-    <row r="21" spans="1:2" s="26" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A21" s="24" t="s">
+      <c r="B20" s="22"/>
+    </row>
+    <row r="21" spans="1:2" s="23" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A21" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="25"/>
+      <c r="B21" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>